<commit_message>
Removed the capability for NPCs and used plain NBT data for them
</commit_message>
<xml_diff>
--- a/entity-balance.xlsx
+++ b/entity-balance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Forge Projects\Mine Mine no Mi - 1.7.10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862F1FCF-4454-4388-95CA-26A38CC64087}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D1DB76-1F4B-4734-AA07-16E7F619B0B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>HP</t>
   </si>
@@ -73,6 +74,15 @@
   </si>
   <si>
     <t>Fat Pirate</t>
+  </si>
+  <si>
+    <t>Player HP :</t>
+  </si>
+  <si>
+    <t>Attack</t>
+  </si>
+  <si>
+    <t>Lapahn Jump</t>
   </si>
 </sst>
 </file>
@@ -140,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -148,13 +158,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -443,13 +456,18 @@
   <dimension ref="B2:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="17" max="17" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
@@ -457,41 +475,55 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="H3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
     <row r="4" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="H4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -510,9 +542,16 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="1">
+        <v>2</v>
+      </c>
+      <c r="J5" s="1">
+        <f>ROUNDDOWN($I$2/I5, 0)</f>
+        <v>20</v>
+      </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -526,14 +565,21 @@
       </c>
       <c r="D6" s="1">
         <f>ROUNDDOWN(C6/$C$2, 0)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="1">
+        <v>6</v>
+      </c>
+      <c r="J6" s="1">
+        <f>ROUNDDOWN($I$2/I6, 0)</f>
+        <v>6</v>
+      </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -547,14 +593,14 @@
       </c>
       <c r="D7" s="1">
         <f>ROUNDDOWN(C7/$C$2, 0)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -566,25 +612,34 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="H8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="1">
+        <v>2</v>
+      </c>
+      <c r="J9" s="1">
+        <f>ROUNDDOWN($I$2/I9, 0)</f>
+        <v>20</v>
+      </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -603,9 +658,16 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="H10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="1">
+        <v>6</v>
+      </c>
+      <c r="J10" s="1">
+        <f>ROUNDDOWN($I$2/I10, 0)</f>
+        <v>6</v>
+      </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
@@ -619,14 +681,21 @@
       </c>
       <c r="D11" s="1">
         <f>ROUNDDOWN(C11/$C$2, 0)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="H11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="1">
+        <v>6</v>
+      </c>
+      <c r="J11" s="1">
+        <f>ROUNDDOWN($I$2/I11, 0)</f>
+        <v>6</v>
+      </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -640,14 +709,14 @@
       </c>
       <c r="D12" s="1">
         <f>ROUNDDOWN(C12/$C$2, 0)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -659,25 +728,34 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="H13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
     <row r="14" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="H14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="1">
+        <v>8</v>
+      </c>
+      <c r="J14" s="1">
+        <f>ROUNDDOWN($I$2/I14, 0)</f>
+        <v>5</v>
+      </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -696,9 +774,16 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="H15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="1">
+        <v>6</v>
+      </c>
+      <c r="J15" s="1">
+        <f>ROUNDDOWN($I$2/I15, 0)</f>
+        <v>6</v>
+      </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -712,14 +797,21 @@
       </c>
       <c r="D16" s="1">
         <f>ROUNDDOWN(C16/$C$2, 0)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="H16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="1">
+        <v>6</v>
+      </c>
+      <c r="J16" s="1">
+        <f>ROUNDDOWN($I$2/I16, 0)</f>
+        <v>6</v>
+      </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
@@ -871,18 +963,18 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H13:J13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>